<commit_message>
Can merge cells in excel files now
</commit_message>
<xml_diff>
--- a/7_19.xlsx
+++ b/7_19.xlsx
@@ -413,14 +413,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="F2:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:I2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TODO set value to cell coordinates
</commit_message>
<xml_diff>
--- a/7_19.xlsx
+++ b/7_19.xlsx
@@ -26,12 +26,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b6d7a8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f9cb9c"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ea9999"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="F2:I2"/>
+  <dimension ref="F2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,10 +439,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2"/>
+    <row r="2">
+      <c r="F2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="F3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="F4" s="3" t="n"/>
+      <c r="J4" s="3" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Can generate correctly spaces colored week cells
</commit_message>
<xml_diff>
--- a/7_19.xlsx
+++ b/7_19.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -48,6 +48,11 @@
         <fgColor rgb="00ea9999"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00cccccc"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -61,11 +66,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -431,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="F2:J4"/>
+  <dimension ref="A2:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,16 +457,133 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
-      <c r="F2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Tillgänglig</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="F3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Krock med icke obligatoriskt moment</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="n"/>
     </row>
     <row r="4">
-      <c r="F4" s="3" t="n"/>
-      <c r="J4" s="3" t="n"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>Krock med obligatoriskt moment</t>
+        </is>
+      </c>
+      <c r="J4" s="6" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 13</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 18</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 19</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Can print all the activities and the corresponding availability cells
</commit_message>
<xml_diff>
--- a/7_19.xlsx
+++ b/7_19.xlsx
@@ -54,7 +54,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,11 +62,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -83,6 +89,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -480,108 +490,1578 @@
       </c>
       <c r="J4" s="6" t="n"/>
     </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 3</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 3</t>
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-17</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="inlineStr">
+        <is>
+          <t>15:15-17:00</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H7" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I7" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-18</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H8" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I8" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-19</t>
+        </is>
+      </c>
+      <c r="B9" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C9" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>Seminarium 1</t>
+        </is>
+      </c>
+      <c r="F9" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G9" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H9" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-20</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C10" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D10" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 4</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 4</t>
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-23</t>
+        </is>
+      </c>
+      <c r="B13" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C13" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F13" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G13" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H13" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-24</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C14" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F14" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G14" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H14" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-25</t>
+        </is>
+      </c>
+      <c r="B15" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C15" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F15" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G15" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H15" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I15" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="B16" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C16" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F16" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G16" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H16" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I16" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-27</t>
+        </is>
+      </c>
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C17" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H17" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I17" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 5</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 5</t>
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
+      <c r="B20" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C20" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>Seminarium 2</t>
+        </is>
+      </c>
+      <c r="F20" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G20" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H20" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I20" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="B21" s="8" t="inlineStr">
+        <is>
+          <t>08:15-12:00</t>
+        </is>
+      </c>
+      <c r="C21" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>Dugga</t>
+        </is>
+      </c>
+      <c r="F21" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G21" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H21" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I21" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-02</t>
+        </is>
+      </c>
+      <c r="B22" s="8" t="inlineStr">
+        <is>
+          <t>08:15-10:00</t>
+        </is>
+      </c>
+      <c r="C22" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F22" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G22" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H22" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I22" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-02</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C23" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F23" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G23" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H23" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I23" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-03</t>
+        </is>
+      </c>
+      <c r="B24" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C24" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D24" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F24" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G24" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H24" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I24" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 6</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 6</t>
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C27" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D27" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F27" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G27" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H27" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I27" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="B28" s="8" t="inlineStr">
+        <is>
+          <t>08:15-10:00</t>
+        </is>
+      </c>
+      <c r="C28" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D28" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F28" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G28" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H28" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I28" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-08</t>
+        </is>
+      </c>
+      <c r="B29" s="8" t="inlineStr">
+        <is>
+          <t>08:15-10:00</t>
+        </is>
+      </c>
+      <c r="C29" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D29" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F29" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G29" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H29" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I29" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-10</t>
+        </is>
+      </c>
+      <c r="B30" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C30" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D30" s="8" t="inlineStr">
+        <is>
+          <t>Seminarium 3</t>
+        </is>
+      </c>
+      <c r="F30" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G30" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H30" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I30" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 7</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 7</t>
+      <c r="A33" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-15</t>
+        </is>
+      </c>
+      <c r="B33" s="8" t="inlineStr">
+        <is>
+          <t>08:15-10:00</t>
+        </is>
+      </c>
+      <c r="C33" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D33" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F33" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G33" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H33" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I33" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-16</t>
+        </is>
+      </c>
+      <c r="B34" s="8" t="inlineStr">
+        <is>
+          <t>08:15-12:00</t>
+        </is>
+      </c>
+      <c r="C34" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D34" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F34" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G34" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H34" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I34" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-16</t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C35" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D35" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F35" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G35" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H35" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I35" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-17</t>
+        </is>
+      </c>
+      <c r="B36" s="8" t="inlineStr">
+        <is>
+          <t>13:15-15:00</t>
+        </is>
+      </c>
+      <c r="C36" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D36" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F36" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G36" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H36" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I36" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 8</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 8</t>
+      <c r="A39" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
+        </is>
+      </c>
+      <c r="B39" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C39" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D39" s="8" t="inlineStr">
+        <is>
+          <t>Laboration</t>
+        </is>
+      </c>
+      <c r="F39" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G39" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H39" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I39" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+      <c r="B40" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C40" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D40" s="8" t="inlineStr">
+        <is>
+          <t>Seminarium 4</t>
+        </is>
+      </c>
+      <c r="F40" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G40" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H40" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I40" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-24</t>
+        </is>
+      </c>
+      <c r="B41" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C41" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D41" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F41" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G41" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H41" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I41" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 9</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 9</t>
+      <c r="A44" s="8" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B44" s="8" t="inlineStr">
+        <is>
+          <t>13:15-17:00</t>
+        </is>
+      </c>
+      <c r="C44" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D44" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F44" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G44" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H44" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I44" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="8" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="B45" s="8" t="inlineStr">
+        <is>
+          <t>08:15-12:00</t>
+        </is>
+      </c>
+      <c r="C45" s="8" t="inlineStr">
+        <is>
+          <t>TDP007</t>
+        </is>
+      </c>
+      <c r="D45" s="8" t="inlineStr">
+        <is>
+          <t>Dugga</t>
+        </is>
+      </c>
+      <c r="F45" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G45" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H45" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I45" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 10</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 10</t>
+      <c r="A48" s="8" t="inlineStr">
+        <is>
+          <t>2023-03-07</t>
+        </is>
+      </c>
+      <c r="B48" s="8" t="inlineStr">
+        <is>
+          <t>13:15-17:00</t>
+        </is>
+      </c>
+      <c r="C48" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D48" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F48" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G48" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H48" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I48" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 13</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 13</t>
+      <c r="A51" s="8" t="inlineStr">
+        <is>
+          <t>2023-03-29</t>
+        </is>
+      </c>
+      <c r="B51" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C51" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D51" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F51" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G51" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H51" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I51" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 14</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 14</t>
+      <c r="A54" s="8" t="inlineStr">
+        <is>
+          <t>2023-04-05</t>
+        </is>
+      </c>
+      <c r="B54" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C54" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D54" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F54" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G54" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H54" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I54" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 15</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 15</t>
+      <c r="A57" s="8" t="inlineStr">
+        <is>
+          <t>2023-04-12</t>
+        </is>
+      </c>
+      <c r="B57" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C57" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D57" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F57" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H57" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I57" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 16</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 16</t>
+      <c r="A60" s="8" t="inlineStr">
+        <is>
+          <t>2023-04-19</t>
+        </is>
+      </c>
+      <c r="B60" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C60" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F60" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G60" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H60" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I60" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 17</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 17</t>
+      <c r="A63" s="8" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="B63" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C63" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F63" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H63" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I63" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 18</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 18</t>
+      <c r="A66" s="8" t="inlineStr">
+        <is>
+          <t>2023-05-03</t>
+        </is>
+      </c>
+      <c r="B66" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C66" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F66" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G66" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H66" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I66" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>Vecka 19</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="7" t="inlineStr">
-        <is>
-          <t>Vecka 19</t>
+      <c r="A69" s="8" t="inlineStr">
+        <is>
+          <t>2023-05-10</t>
+        </is>
+      </c>
+      <c r="B69" s="8" t="inlineStr">
+        <is>
+          <t>10:15-12:00</t>
+        </is>
+      </c>
+      <c r="C69" s="8" t="inlineStr">
+        <is>
+          <t>TDP019</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>Handledning</t>
+        </is>
+      </c>
+      <c r="F69" s="9" t="inlineStr">
+        <is>
+          <t>Aron</t>
+        </is>
+      </c>
+      <c r="G69" s="9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="H69" s="9" t="inlineStr">
+        <is>
+          <t>Mattias</t>
+        </is>
+      </c>
+      <c r="I69" s="9" t="inlineStr">
+        <is>
+          <t>Sopi</t>
         </is>
       </c>
     </row>

</xml_diff>